<commit_message>
Changes after implementing local time + table of errors
</commit_message>
<xml_diff>
--- a/Projects/AireAD/Andorra_info.xlsx
+++ b/Projects/AireAD/Andorra_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\4sfera_local\Projectes\Andorra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EE0D51-5228-444C-A47C-FB779B3BE798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AD05E5-853F-4CF6-A56D-D7EFD77D5CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" tabRatio="801" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -964,9 +964,6 @@
     <t>moreinfo_url</t>
   </si>
   <si>
-    <t>http://www.aire.ad/moreinfo.php?n_action=impacts&amp;t=2#inversion</t>
-  </si>
-  <si>
     <t>SR</t>
   </si>
   <si>
@@ -1334,6 +1331,9 @@
   </si>
   <si>
     <t>Actualment hi ha condicions d'inversi&amp;oacute; t&amp;egrave;rmica</t>
+  </si>
+  <si>
+    <t>http://www.aire.ad/about_air/air_atmospheric_phenomena?jumpTo=thermalInversion</t>
   </si>
 </sst>
 </file>
@@ -3605,7 +3605,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B1" t="s">
         <v>21</v>
@@ -3628,7 +3628,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3651,7 +3651,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -3674,7 +3674,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3697,7 +3697,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -3720,7 +3720,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3743,7 +3743,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3781,52 +3781,52 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -3850,108 +3850,108 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B9" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -3977,13 +3977,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D1" t="s">
         <v>157</v>
@@ -3991,366 +3991,366 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B2" t="s">
         <v>370</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D2" t="s">
         <v>371</v>
-      </c>
-      <c r="C2" t="s">
-        <v>371</v>
-      </c>
-      <c r="D2" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>372</v>
+      </c>
+      <c r="B3" t="s">
         <v>373</v>
       </c>
-      <c r="B3" t="s">
-        <v>374</v>
-      </c>
       <c r="C3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>374</v>
+      </c>
+      <c r="B4" t="s">
         <v>375</v>
       </c>
-      <c r="B4" t="s">
-        <v>376</v>
-      </c>
       <c r="C4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>376</v>
+      </c>
+      <c r="B5" t="s">
         <v>377</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>378</v>
       </c>
-      <c r="C5" t="s">
-        <v>379</v>
-      </c>
       <c r="D5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>379</v>
+      </c>
+      <c r="B6" t="s">
         <v>380</v>
       </c>
-      <c r="B6" t="s">
-        <v>381</v>
-      </c>
       <c r="C6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>381</v>
+      </c>
+      <c r="B7" t="s">
         <v>382</v>
       </c>
-      <c r="B7" t="s">
-        <v>383</v>
-      </c>
       <c r="C7" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>383</v>
+      </c>
+      <c r="B8" t="s">
         <v>384</v>
       </c>
-      <c r="B8" t="s">
-        <v>385</v>
-      </c>
       <c r="C8" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>385</v>
+      </c>
+      <c r="B9" t="s">
         <v>386</v>
       </c>
-      <c r="B9" t="s">
-        <v>387</v>
-      </c>
       <c r="C9" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D9" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>387</v>
+      </c>
+      <c r="B10" t="s">
         <v>388</v>
       </c>
-      <c r="B10" t="s">
-        <v>389</v>
-      </c>
       <c r="C10" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>389</v>
+      </c>
+      <c r="B11" t="s">
         <v>390</v>
       </c>
-      <c r="B11" t="s">
-        <v>391</v>
-      </c>
       <c r="C11" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D11" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>391</v>
+      </c>
+      <c r="B12" t="s">
         <v>392</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>393</v>
       </c>
-      <c r="C12" t="s">
-        <v>394</v>
-      </c>
       <c r="D12" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>394</v>
+      </c>
+      <c r="B13" t="s">
         <v>395</v>
       </c>
-      <c r="B13" t="s">
-        <v>396</v>
-      </c>
       <c r="C13" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>396</v>
+      </c>
+      <c r="B14" t="s">
         <v>397</v>
       </c>
-      <c r="B14" t="s">
-        <v>398</v>
-      </c>
       <c r="C14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D14" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>398</v>
+      </c>
+      <c r="B15" t="s">
         <v>399</v>
       </c>
-      <c r="B15" t="s">
-        <v>400</v>
-      </c>
       <c r="C15" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D15" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>400</v>
+      </c>
+      <c r="B16" t="s">
         <v>401</v>
       </c>
-      <c r="B16" t="s">
-        <v>402</v>
-      </c>
       <c r="C16" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D16" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>402</v>
+      </c>
+      <c r="B17" t="s">
         <v>403</v>
       </c>
-      <c r="B17" t="s">
-        <v>404</v>
-      </c>
       <c r="C17" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>404</v>
+      </c>
+      <c r="B18" t="s">
         <v>405</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>406</v>
       </c>
-      <c r="C18" t="s">
-        <v>407</v>
-      </c>
       <c r="D18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>407</v>
+      </c>
+      <c r="B19" t="s">
         <v>408</v>
       </c>
-      <c r="B19" t="s">
-        <v>409</v>
-      </c>
       <c r="C19" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D19" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>409</v>
+      </c>
+      <c r="B20" t="s">
         <v>410</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>411</v>
       </c>
-      <c r="C20" t="s">
-        <v>412</v>
-      </c>
       <c r="D20" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>412</v>
+      </c>
+      <c r="B21" t="s">
         <v>413</v>
       </c>
-      <c r="B21" t="s">
-        <v>414</v>
-      </c>
       <c r="C21" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D21" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B22" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C22" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D22" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>415</v>
+      </c>
+      <c r="B23" t="s">
         <v>416</v>
       </c>
-      <c r="B23" t="s">
-        <v>417</v>
-      </c>
       <c r="C23" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D23" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>417</v>
+      </c>
+      <c r="B24" t="s">
         <v>418</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>419</v>
       </c>
-      <c r="C24" t="s">
-        <v>420</v>
-      </c>
       <c r="D24" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B25" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C25" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D25" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>421</v>
+      </c>
+      <c r="B26" t="s">
         <v>422</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>423</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>424</v>
-      </c>
-      <c r="D26" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B27" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C27" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D27" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
   </sheetData>
@@ -4402,7 +4402,7 @@
         <v>154</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>150</v>
@@ -4440,7 +4440,7 @@
         <v>155</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>151</v>
@@ -4475,7 +4475,7 @@
         <v>155</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>151</v>
@@ -4510,7 +4510,7 @@
         <v>155</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>151</v>
@@ -4545,7 +4545,7 @@
         <v>155</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>151</v>
@@ -4615,7 +4615,7 @@
         <v>155</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>151</v>
@@ -4650,7 +4650,7 @@
         <v>184</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>151</v>
@@ -4723,7 +4723,7 @@
         <v>185</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>151</v>
@@ -4930,7 +4930,7 @@
         <v>155</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>153</v>
@@ -4965,7 +4965,7 @@
         <v>155</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>153</v>
@@ -5000,7 +5000,7 @@
         <v>155</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>153</v>
@@ -5035,7 +5035,7 @@
         <v>155</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>153</v>
@@ -5535,13 +5535,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>
@@ -5595,7 +5595,7 @@
         <v>154</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>234</v>
@@ -5639,7 +5639,7 @@
         <v>155</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>151</v>
@@ -5680,7 +5680,7 @@
         <v>155</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>151</v>
@@ -5715,13 +5715,13 @@
         <v>28</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F4" s="7" t="s">
         <v>155</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>151</v>
@@ -5762,7 +5762,7 @@
         <v>155</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>151</v>
@@ -5844,7 +5844,7 @@
         <v>155</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>151</v>
@@ -5885,7 +5885,7 @@
         <v>184</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>151</v>
@@ -5970,7 +5970,7 @@
         <v>185</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>151</v>
@@ -6125,10 +6125,10 @@
         <v>14</v>
       </c>
       <c r="D14" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>308</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>309</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>186</v>
@@ -6149,10 +6149,10 @@
         <v>177</v>
       </c>
       <c r="L14" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="M14" s="11" t="s">
         <v>310</v>
-      </c>
-      <c r="M14" s="11" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -6216,7 +6216,7 @@
         <v>155</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>153</v>
@@ -6257,7 +6257,7 @@
         <v>155</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>153</v>
@@ -6298,7 +6298,7 @@
         <v>155</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>153</v>
@@ -6339,7 +6339,7 @@
         <v>155</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>153</v>
@@ -6392,7 +6392,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -6450,14 +6450,14 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>307</v>
+      <c r="A2" s="11" t="s">
+        <v>430</v>
       </c>
       <c r="B2" t="s">
+        <v>428</v>
+      </c>
+      <c r="C2" t="s">
         <v>429</v>
-      </c>
-      <c r="C2" t="s">
-        <v>430</v>
       </c>
       <c r="D2" t="s">
         <v>301</v>
@@ -6478,25 +6478,28 @@
         <v>305</v>
       </c>
       <c r="J2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="K2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="M2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="N2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="O2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{6FB1A650-2E03-46B1-8DD1-89AFB43AE9B8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6676,16 +6679,16 @@
         <v>171</v>
       </c>
       <c r="E1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F1" t="s">
         <v>136</v>
       </c>
       <c r="G1" t="s">
+        <v>317</v>
+      </c>
+      <c r="H1" t="s">
         <v>318</v>
-      </c>
-      <c r="H1" t="s">
-        <v>319</v>
       </c>
       <c r="I1" t="s">
         <v>157</v>
@@ -6750,10 +6753,10 @@
         <v>139</v>
       </c>
       <c r="D2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F2" t="s">
         <v>93</v>
@@ -6762,7 +6765,7 @@
         <v>38692</v>
       </c>
       <c r="H2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I2" t="s">
         <v>94</v>
@@ -6827,10 +6830,10 @@
         <v>100</v>
       </c>
       <c r="D3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F3" t="s">
         <v>100</v>
@@ -6839,7 +6842,7 @@
         <v>38487</v>
       </c>
       <c r="H3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I3" t="s">
         <v>101</v>
@@ -6916,7 +6919,7 @@
         <v>38353</v>
       </c>
       <c r="H4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I4" t="s">
         <v>94</v>
@@ -6981,7 +6984,7 @@
         <v>39045</v>
       </c>
       <c r="H5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I5" t="s">
         <v>111</v>
@@ -7037,7 +7040,7 @@
         <v>162</v>
       </c>
       <c r="E6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F6" t="s">
         <v>114</v>
@@ -7110,7 +7113,7 @@
         <v>199</v>
       </c>
       <c r="E7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F7" t="s">
         <v>141</v>
@@ -7119,7 +7122,7 @@
         <v>40003</v>
       </c>
       <c r="H7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I7" t="s">
         <v>111</v>
@@ -7325,19 +7328,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>313</v>
+      </c>
+      <c r="C7" t="s">
+        <v>313</v>
+      </c>
+      <c r="D7" t="s">
         <v>314</v>
       </c>
-      <c r="C7" t="s">
-        <v>314</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>315</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>316</v>
-      </c>
-      <c r="F7" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -7345,19 +7348,19 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
+        <v>322</v>
+      </c>
+      <c r="C8" t="s">
+        <v>322</v>
+      </c>
+      <c r="D8" t="s">
         <v>323</v>
       </c>
-      <c r="C8" t="s">
-        <v>323</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>324</v>
       </c>
-      <c r="E8" t="s">
-        <v>325</v>
-      </c>
       <c r="F8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>